<commit_message>
Mankind Automation - Question 1
</commit_message>
<xml_diff>
--- a/src/main/java/com/testData/FormTestData.xlsx
+++ b/src/main/java/com/testData/FormTestData.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenabler\SelenablerFramework-baseline-SelenablerWithJira_New\src\main\java\com\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test Domain\3_Office_Training\SelenablerFramework\Selenium-hands-on\src\main\java\com\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1630FABF-5222-4E18-B1C1-17B6E8758582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{2A0C6CEF-72F9-44FD-BABA-22BED32905E2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="DropdownNames" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="Columns" sheetId="3" r:id="rId3"/>
+    <sheet name="Data" r:id="rId1" sheetId="1"/>
+    <sheet name="DropdownNames" r:id="rId2" sheetId="2" state="hidden"/>
+    <sheet name="Columns" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
   <si>
     <t>noOfRecords</t>
   </si>
@@ -183,16 +183,94 @@
   </si>
   <si>
     <t>100</t>
+  </si>
+  <si>
+    <t>Swaraj Purekar</t>
+  </si>
+  <si>
+    <t>Suraj@12345</t>
+  </si>
+  <si>
+    <t>fullname</t>
+  </si>
+  <si>
+    <t>validEmail</t>
+  </si>
+  <si>
+    <t>invalidEmail</t>
+  </si>
+  <si>
+    <t>Swa@@gmailcom</t>
+  </si>
+  <si>
+    <t>validPassword</t>
+  </si>
+  <si>
+    <t>invalidPassword</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>swaraz2@gmail.com</t>
+  </si>
+  <si>
+    <t>Tanmayyyy@123456</t>
+  </si>
+  <si>
+    <t>swaraz3@gmail.com</t>
+  </si>
+  <si>
+    <t>swaraz4@gmail.com</t>
+  </si>
+  <si>
+    <t>swaraz5@gmail.com</t>
+  </si>
+  <si>
+    <t>swaraz6@gmail.com</t>
+  </si>
+  <si>
+    <t>swaraz7@gmail.com</t>
+  </si>
+  <si>
+    <t>swaraz8@gmail.com</t>
+  </si>
+  <si>
+    <t>swaraz9@gmail.com</t>
+  </si>
+  <si>
+    <t>swaraz10@gmail.com</t>
+  </si>
+  <si>
+    <t>swaraz11@gmail.com</t>
+  </si>
+  <si>
+    <t>swaraz12@gmail.com</t>
+  </si>
+  <si>
+    <t>swaraz13@gmail.com</t>
+  </si>
+  <si>
+    <t>swaraz14@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,18 +293,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -243,10 +326,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -281,7 +364,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -316,7 +399,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -410,21 +493,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -441,7 +524,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -493,27 +576,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="52.90625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +604,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -529,7 +612,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -537,7 +620,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -545,7 +628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -553,7 +636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -561,7 +644,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -569,7 +652,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -577,7 +660,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -585,7 +668,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -593,7 +676,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -601,212 +684,264 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="4">
+        <v>7562348899</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B15" xr:uid="{0B1199A7-ACCA-461D-BE6C-9A750C9FB4E3}"/>
+    <hyperlink display="swaraz@gmail.com" r:id="rId2" ref="B13" xr:uid="{F4D58E92-D37D-4FDE-83E7-17D6CFCA7D30}"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6554FA4C-6261-4A9A-A432-234693BB3C16}">
-  <dimension ref="A1:A30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6554FA4C-6261-4A9A-A432-234693BB3C16}">
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206D7B4F-8D7A-4AFD-A5A7-6C692A0A91C8}">
-  <dimension ref="A1:R2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206D7B4F-8D7A-4AFD-A5A7-6C692A0A91C8}">
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7265625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
+    <col min="14" max="15" bestFit="true" customWidth="true" width="22.26953125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -862,7 +997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -919,11 +1054,11 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A98028FE-F85A-4937-8C41-3624A56FE2CF}">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{A98028FE-F85A-4937-8C41-3624A56FE2CF}">
           <x14:formula1>
             <xm:f>DropdownNames!$A$1:$A$30</xm:f>
           </x14:formula1>

</xml_diff>